<commit_message>
new code ... change time delete
</commit_message>
<xml_diff>
--- a/export/alarm_2024-11-19.xlsx
+++ b/export/alarm_2024-11-19.xlsx
@@ -397,401 +397,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>id</v>
+        <v>sensor</v>
       </c>
       <c r="B1" t="str">
-        <v>timestamp</v>
+        <v>sensor_state</v>
       </c>
       <c r="C1" t="str">
-        <v>sensor</v>
+        <v>acknowledgment_state</v>
       </c>
       <c r="D1" t="str">
-        <v>sensor_state</v>
+        <v>alarm_class</v>
       </c>
       <c r="E1" t="str">
-        <v>acknowledgment_state</v>
+        <v>priority</v>
       </c>
       <c r="F1" t="str">
-        <v>alarm_class</v>
+        <v>message</v>
       </c>
       <c r="G1" t="str">
         <v>status</v>
       </c>
       <c r="H1" t="str">
-        <v>priority</v>
+        <v>formatted_timestamp</v>
       </c>
       <c r="I1" t="str">
-        <v>message</v>
-      </c>
-      <c r="J1" t="str">
-        <v>change_timestamps</v>
-      </c>
-      <c r="K1" t="str">
-        <v>formatted_timestamp</v>
+        <v>timestamp</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>21</v>
+      <c r="A2" t="str">
+        <v>thanhtung4</v>
       </c>
       <c r="B2" t="str">
+        <v>active</v>
+      </c>
+      <c r="C2" t="str">
+        <v>none</v>
+      </c>
+      <c r="D2" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G2" t="str">
+        <v>new</v>
+      </c>
+      <c r="H2" t="str">
         <v>2024-11-19 18:00:51</v>
       </c>
-      <c r="C2" t="str">
-        <v>thanhtung4</v>
-      </c>
-      <c r="D2" t="str">
-        <v>active</v>
-      </c>
-      <c r="E2" t="str">
-        <v>none</v>
-      </c>
-      <c r="F2" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G2" t="str">
-        <v>new</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K2" t="str">
         <v>2024-11-19 18:00:51</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
-        <v>22</v>
+      <c r="A3" t="str">
+        <v>thanhtung6</v>
       </c>
       <c r="B3" t="str">
+        <v>active</v>
+      </c>
+      <c r="C3" t="str">
+        <v>none</v>
+      </c>
+      <c r="D3" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G3" t="str">
+        <v>new</v>
+      </c>
+      <c r="H3" t="str">
         <v>2024-11-19 18:00:57</v>
       </c>
-      <c r="C3" t="str">
-        <v>thanhtung6</v>
-      </c>
-      <c r="D3" t="str">
-        <v>active</v>
-      </c>
-      <c r="E3" t="str">
-        <v>none</v>
-      </c>
-      <c r="F3" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G3" t="str">
-        <v>new</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="I3" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K3" t="str">
         <v>2024-11-19 18:00:57</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
-        <v>23</v>
+      <c r="A4" t="str">
+        <v>thanhtung7</v>
       </c>
       <c r="B4" t="str">
+        <v>active</v>
+      </c>
+      <c r="C4" t="str">
+        <v>none</v>
+      </c>
+      <c r="D4" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G4" t="str">
+        <v>new</v>
+      </c>
+      <c r="H4" t="str">
         <v>2024-11-19 18:01:05</v>
       </c>
-      <c r="C4" t="str">
-        <v>thanhtung7</v>
-      </c>
-      <c r="D4" t="str">
-        <v>active</v>
-      </c>
-      <c r="E4" t="str">
-        <v>none</v>
-      </c>
-      <c r="F4" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G4" t="str">
-        <v>new</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K4" t="str">
         <v>2024-11-19 18:01:05</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
-        <v>24</v>
+      <c r="A5" t="str">
+        <v>thanhtung8</v>
       </c>
       <c r="B5" t="str">
+        <v>active</v>
+      </c>
+      <c r="C5" t="str">
+        <v>none</v>
+      </c>
+      <c r="D5" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G5" t="str">
+        <v>new</v>
+      </c>
+      <c r="H5" t="str">
         <v>2024-11-19 18:01:10</v>
       </c>
-      <c r="C5" t="str">
-        <v>thanhtung8</v>
-      </c>
-      <c r="D5" t="str">
-        <v>active</v>
-      </c>
-      <c r="E5" t="str">
-        <v>none</v>
-      </c>
-      <c r="F5" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G5" t="str">
-        <v>new</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
       <c r="I5" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K5" t="str">
         <v>2024-11-19 18:01:10</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
-        <v>25</v>
+      <c r="A6" t="str">
+        <v>thanhtung9</v>
       </c>
       <c r="B6" t="str">
+        <v>active</v>
+      </c>
+      <c r="C6" t="str">
+        <v>none</v>
+      </c>
+      <c r="D6" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G6" t="str">
+        <v>new</v>
+      </c>
+      <c r="H6" t="str">
         <v>2024-11-19 18:01:15</v>
       </c>
-      <c r="C6" t="str">
-        <v>thanhtung9</v>
-      </c>
-      <c r="D6" t="str">
-        <v>active</v>
-      </c>
-      <c r="E6" t="str">
-        <v>none</v>
-      </c>
-      <c r="F6" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G6" t="str">
-        <v>new</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="I6" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K6" t="str">
         <v>2024-11-19 18:01:15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
-        <v>26</v>
+      <c r="A7" t="str">
+        <v>thanhtun19</v>
       </c>
       <c r="B7" t="str">
+        <v>active</v>
+      </c>
+      <c r="C7" t="str">
+        <v>none</v>
+      </c>
+      <c r="D7" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G7" t="str">
+        <v>new</v>
+      </c>
+      <c r="H7" t="str">
         <v>2024-11-19 18:01:19</v>
       </c>
-      <c r="C7" t="str">
-        <v>thanhtun19</v>
-      </c>
-      <c r="D7" t="str">
-        <v>active</v>
-      </c>
-      <c r="E7" t="str">
-        <v>none</v>
-      </c>
-      <c r="F7" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G7" t="str">
-        <v>new</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="I7" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K7" t="str">
         <v>2024-11-19 18:01:19</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
-        <v>27</v>
+      <c r="A8" t="str">
+        <v>thanhtun29</v>
       </c>
       <c r="B8" t="str">
+        <v>active</v>
+      </c>
+      <c r="C8" t="str">
+        <v>none</v>
+      </c>
+      <c r="D8" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G8" t="str">
+        <v>new</v>
+      </c>
+      <c r="H8" t="str">
         <v>2024-11-19 18:01:23</v>
       </c>
-      <c r="C8" t="str">
-        <v>thanhtun29</v>
-      </c>
-      <c r="D8" t="str">
-        <v>active</v>
-      </c>
-      <c r="E8" t="str">
-        <v>none</v>
-      </c>
-      <c r="F8" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G8" t="str">
-        <v>new</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
       <c r="I8" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K8" t="str">
         <v>2024-11-19 18:01:23</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
-        <v>28</v>
+      <c r="A9" t="str">
+        <v>thanhtun39</v>
       </c>
       <c r="B9" t="str">
+        <v>active</v>
+      </c>
+      <c r="C9" t="str">
+        <v>none</v>
+      </c>
+      <c r="D9" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G9" t="str">
+        <v>new</v>
+      </c>
+      <c r="H9" t="str">
         <v>2024-11-19 18:01:27</v>
       </c>
-      <c r="C9" t="str">
-        <v>thanhtun39</v>
-      </c>
-      <c r="D9" t="str">
-        <v>active</v>
-      </c>
-      <c r="E9" t="str">
-        <v>none</v>
-      </c>
-      <c r="F9" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G9" t="str">
-        <v>new</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
       <c r="I9" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K9" t="str">
         <v>2024-11-19 18:01:27</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
-        <v>29</v>
+      <c r="A10" t="str">
+        <v>thanhtun49</v>
       </c>
       <c r="B10" t="str">
+        <v>active</v>
+      </c>
+      <c r="C10" t="str">
+        <v>none</v>
+      </c>
+      <c r="D10" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G10" t="str">
+        <v>new</v>
+      </c>
+      <c r="H10" t="str">
         <v>2024-11-19 18:01:31</v>
       </c>
-      <c r="C10" t="str">
-        <v>thanhtun49</v>
-      </c>
-      <c r="D10" t="str">
-        <v>active</v>
-      </c>
-      <c r="E10" t="str">
-        <v>none</v>
-      </c>
-      <c r="F10" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G10" t="str">
-        <v>new</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="I10" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K10" t="str">
         <v>2024-11-19 18:01:31</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
-        <v>30</v>
+      <c r="A11" t="str">
+        <v>thanhtun59</v>
       </c>
       <c r="B11" t="str">
+        <v>active</v>
+      </c>
+      <c r="C11" t="str">
+        <v>none</v>
+      </c>
+      <c r="D11" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G11" t="str">
+        <v>new</v>
+      </c>
+      <c r="H11" t="str">
         <v>2024-11-19 18:01:35</v>
       </c>
-      <c r="C11" t="str">
-        <v>thanhtun59</v>
-      </c>
-      <c r="D11" t="str">
-        <v>active</v>
-      </c>
-      <c r="E11" t="str">
-        <v>none</v>
-      </c>
-      <c r="F11" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G11" t="str">
-        <v>new</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
       <c r="I11" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K11" t="str">
         <v>2024-11-19 18:01:35</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
-        <v>31</v>
+      <c r="A12" t="str">
+        <v>thanhtun69</v>
       </c>
       <c r="B12" t="str">
+        <v>active</v>
+      </c>
+      <c r="C12" t="str">
+        <v>none</v>
+      </c>
+      <c r="D12" t="str">
+        <v>warning</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="str">
+        <v>2D.PP-CBS-DL2.2 disconect.</v>
+      </c>
+      <c r="G12" t="str">
+        <v>new</v>
+      </c>
+      <c r="H12" t="str">
         <v>2024-11-19 23:17:28</v>
       </c>
-      <c r="C12" t="str">
-        <v>thanhtun69</v>
-      </c>
-      <c r="D12" t="str">
-        <v>active</v>
-      </c>
-      <c r="E12" t="str">
-        <v>none</v>
-      </c>
-      <c r="F12" t="str">
-        <v>warning</v>
-      </c>
-      <c r="G12" t="str">
-        <v>new</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
       <c r="I12" t="str">
-        <v>2D.PP-CBS-DL2.2 disconect.</v>
-      </c>
-      <c r="K12" t="str">
         <v>2024-11-19 23:17:28</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>